<commit_message>
BAP projesi yük ile ilgili son çalışmalar ve sipariş aşaması.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="General Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="Figures" sheetId="5" r:id="rId3"/>
-    <sheet name="Not used-old" sheetId="3" r:id="rId4"/>
+    <sheet name="Load design" sheetId="6" r:id="rId3"/>
+    <sheet name="Figures" sheetId="5" r:id="rId4"/>
+    <sheet name="Not used-old" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -127,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="274">
   <si>
     <t>Power factor</t>
   </si>
@@ -1896,6 +1897,341 @@
   </si>
   <si>
     <t>Peak Tooth Flux</t>
+  </si>
+  <si>
+    <t>Input Parameters</t>
+  </si>
+  <si>
+    <t>Total drive output power</t>
+  </si>
+  <si>
+    <t>Calculated parameters</t>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>outd</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>dc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>drm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>dcm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>r</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>η</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>m</t>
+    </r>
+  </si>
+  <si>
+    <t>Drive apparent power (module)</t>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>drm</t>
+    </r>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Phase resistance/module</t>
+  </si>
+  <si>
+    <t>Phase impedance/module</t>
+  </si>
+  <si>
+    <r>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Ω</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase reactance/module</t>
+  </si>
+  <si>
+    <r>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>Phase inductance/module</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>phm</t>
+    </r>
+  </si>
+  <si>
+    <t>mH</t>
+  </si>
+  <si>
+    <t>Single resistance</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Number of parallel branches</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Single inductance</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Voltage on Rphm</t>
+  </si>
+  <si>
+    <t>Voltage on Xphm</t>
+  </si>
+  <si>
+    <t>Drive reactive power (module)</t>
+  </si>
+  <si>
+    <r>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+        <charset val="162"/>
+      </rPr>
+      <t>drm</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1906,7 +2242,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2010,6 +2346,29 @@
       <family val="2"/>
       <charset val="162"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2139,7 +2498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2302,6 +2661,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2320,8 +2682,56 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2763,7 +3173,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F2" sqref="F2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2859,7 +3269,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="7">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>15</v>
@@ -2915,14 +3325,14 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="58" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>38</v>
       </c>
       <c r="C6" s="20">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>15</v>
@@ -2951,12 +3361,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -3108,7 +3518,7 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="58" t="s">
         <v>88</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -3148,7 +3558,7 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="58" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="20" t="s">
@@ -3186,8 +3596,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3217,35 +3627,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62" t="s">
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="59" t="s">
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="62"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3366,11 +3776,11 @@
       </c>
       <c r="T3" s="23">
         <f>M7</f>
-        <v>9.7177314523144265</v>
+        <v>8.7459583070829847</v>
       </c>
       <c r="U3" s="23">
         <f>100*ABS(S3-T3)/T3</f>
-        <v>54.357012988124097</v>
+        <v>71.507792209026761</v>
       </c>
       <c r="V3" s="20"/>
     </row>
@@ -3397,7 +3807,7 @@
       </c>
       <c r="H4" s="23">
         <f>SQRT(4*M7/(Parameters!H8*Parameters!C13))</f>
-        <v>1.7587637692667544</v>
+        <v>1.6685098131197376</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>80</v>
@@ -3467,7 +3877,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="64" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -3534,7 +3944,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="63"/>
+      <c r="J6" s="64"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -3543,7 +3953,7 @@
       </c>
       <c r="M6" s="23">
         <f>0.612*Parameters!C6*M5/SQRT(3)</f>
-        <v>81.091154708759703</v>
+        <v>95.401358480893776</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>33</v>
@@ -3609,7 +4019,7 @@
       </c>
       <c r="M7" s="23">
         <f>M4/(Parameters!H3*'General Calculations'!M6*3)</f>
-        <v>9.7177314523144265</v>
+        <v>8.7459583070829847</v>
       </c>
       <c r="N7" s="20" t="s">
         <v>22</v>
@@ -3630,11 +4040,11 @@
       </c>
       <c r="T7" s="23">
         <f>H22</f>
-        <v>75.503284847670415</v>
+        <v>61.157660726613045</v>
       </c>
       <c r="U7" s="23">
         <f t="shared" si="0"/>
-        <v>365.27776997882376</v>
+        <v>474.41699997385632</v>
       </c>
       <c r="V7" s="20"/>
     </row>
@@ -3761,20 +4171,20 @@
       <c r="E10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62" t="s">
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="62"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -3839,7 +4249,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="63" t="s">
+      <c r="O11" s="64" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -3906,7 +4316,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="63"/>
+      <c r="O12" s="64"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -3972,7 +4382,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="63"/>
+      <c r="O13" s="64"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -4137,13 +4547,13 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="62" t="s">
+      <c r="F17" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
       <c r="K17" s="29" t="s">
         <v>140</v>
       </c>
@@ -4283,7 +4693,7 @@
       </c>
       <c r="H20" s="20">
         <f>M7^2*H19/1000</f>
-        <v>6.2919404039725348</v>
+        <v>5.0964717272177538</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>7</v>
@@ -4360,7 +4770,7 @@
       </c>
       <c r="H22" s="20">
         <f>H20*Parameters!C4*Parameters!C7+H21</f>
-        <v>75.503284847670415</v>
+        <v>61.157660726613045</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>7</v>
@@ -4376,19 +4786,19 @@
       </c>
       <c r="H23" s="20">
         <f>Parameters!C2/(Parameters!C2+'General Calculations'!H22)*100</f>
-        <v>99.065033073674314</v>
+        <v>99.241329058423347</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="46"/>
-      <c r="K23" s="62" t="s">
+      <c r="K23" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="44"/>
@@ -4672,6 +5082,470 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" style="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="76" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="76" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="76" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" style="76" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="76" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="76" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5703125" style="76" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" style="76" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="75"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="78" t="s">
+        <v>238</v>
+      </c>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+    </row>
+    <row r="2" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="69">
+        <v>8000</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="67"/>
+      <c r="F2" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>240</v>
+      </c>
+      <c r="H2" s="67">
+        <f>C4/C5</f>
+        <v>2</v>
+      </c>
+      <c r="I2" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="67"/>
+    </row>
+    <row r="3" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="67">
+        <v>540</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="67"/>
+      <c r="F3" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>242</v>
+      </c>
+      <c r="H3" s="69">
+        <f>C2/C4</f>
+        <v>2000</v>
+      </c>
+      <c r="I3" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="67"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="67">
+        <v>4</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="79" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" s="67" t="s">
+        <v>251</v>
+      </c>
+      <c r="H4" s="69">
+        <f>H3/C9</f>
+        <v>2298.8505747126437</v>
+      </c>
+      <c r="I4" s="67" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="67"/>
+    </row>
+    <row r="5" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="67">
+        <v>2</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="67"/>
+      <c r="F5" s="79" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>273</v>
+      </c>
+      <c r="H5" s="69">
+        <f>SQRT(H4^2-H3^2)</f>
+        <v>1133.4522331605565</v>
+      </c>
+      <c r="I5" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="67"/>
+    </row>
+    <row r="6" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="67" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="67">
+        <v>1</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="67"/>
+      <c r="F6" s="79" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>243</v>
+      </c>
+      <c r="H6" s="67">
+        <f>C3/C5</f>
+        <v>270</v>
+      </c>
+      <c r="I6" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="67"/>
+    </row>
+    <row r="7" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="67">
+        <v>3</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="67"/>
+      <c r="F7" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="68">
+        <f>0.612*C6*H6/SQRT(3)</f>
+        <v>95.401358480893776</v>
+      </c>
+      <c r="I7" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="67"/>
+    </row>
+    <row r="8" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="67" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="67">
+        <v>94</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="67"/>
+      <c r="F8" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>247</v>
+      </c>
+      <c r="H8" s="68">
+        <f>H4/(C7*H7)</f>
+        <v>8.0322076866198895</v>
+      </c>
+      <c r="I8" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="67"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="67">
+        <v>0.87</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="67"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="67"/>
+    </row>
+    <row r="10" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="67">
+        <v>50</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="67"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+    </row>
+    <row r="11" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" s="67" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="67">
+        <v>5</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="67"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+    </row>
+    <row r="12" spans="1:10" s="77" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="70" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="65" t="s">
+        <v>256</v>
+      </c>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="70"/>
+    </row>
+    <row r="13" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="68">
+        <f>H7/H8</f>
+        <v>11.877352056000003</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="67"/>
+      <c r="F13" s="81" t="s">
+        <v>270</v>
+      </c>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68">
+        <f>C14*H8</f>
+        <v>82.999181878377584</v>
+      </c>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+    </row>
+    <row r="14" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="74" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="68">
+        <f>C13*C9</f>
+        <v>10.333296288720003</v>
+      </c>
+      <c r="D14" s="67" t="s">
+        <v>257</v>
+      </c>
+      <c r="E14" s="67"/>
+      <c r="F14" s="81" t="s">
+        <v>271</v>
+      </c>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68">
+        <f>C15*H8</f>
+        <v>47.037804025273118</v>
+      </c>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+    </row>
+    <row r="15" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="74" t="s">
+        <v>259</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="68">
+        <f>SQRT(C13^2-C14^2)</f>
+        <v>5.8561488771796872</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>257</v>
+      </c>
+      <c r="E15" s="67"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="74" t="s">
+        <v>261</v>
+      </c>
+      <c r="B16" s="67" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" s="68">
+        <f>1000*C15/(2*3.14*C10)</f>
+        <v>18.650155659807922</v>
+      </c>
+      <c r="D16" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="E16" s="67"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+    </row>
+    <row r="17" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" s="67" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" s="68">
+        <f>C14*C11</f>
+        <v>51.66648144360002</v>
+      </c>
+      <c r="D17" s="67" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="67"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+    </row>
+    <row r="18" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="B18" s="67" t="s">
+        <v>269</v>
+      </c>
+      <c r="C18" s="68">
+        <f>C16*C11</f>
+        <v>93.250778299039609</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>263</v>
+      </c>
+      <c r="E18" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="F12:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="H4" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B1"/>
@@ -4728,7 +5602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R36"/>
@@ -4997,7 +5871,7 @@
       </c>
       <c r="C10" s="8">
         <f>0.612*Parameters!C6*C9/SQRT(3)</f>
-        <v>81.091154708759703</v>
+        <v>95.401358480893776</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>33</v>
@@ -5012,7 +5886,7 @@
       </c>
       <c r="C11" s="8">
         <f>C8/(Parameters!H3*'Not used-old'!C10*3)</f>
-        <v>9.7177314523144265</v>
+        <v>8.7459583070829847</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Design file big progress.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27480" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -2371,7 +2371,7 @@
       <charset val="162"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2417,6 +2417,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2498,7 +2510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2612,12 +2624,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2664,6 +2670,45 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2682,55 +2727,28 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3173,7 +3191,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:I3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3198,16 +3216,16 @@
       <c r="A1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="48"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
@@ -3325,7 +3343,7 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -3337,7 +3355,7 @@
       <c r="D6" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="51" t="s">
         <v>178</v>
       </c>
       <c r="F6" s="6"/>
@@ -3361,12 +3379,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="70" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -3435,7 +3453,7 @@
       <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="50" t="s">
         <v>223</v>
       </c>
       <c r="F10" s="6" t="s">
@@ -3518,7 +3536,7 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="56" t="s">
         <v>88</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -3530,7 +3548,7 @@
       <c r="D14" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="53" t="s">
+      <c r="E14" s="51" t="s">
         <v>178</v>
       </c>
       <c r="F14" s="6"/>
@@ -3558,7 +3576,7 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="36" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="20" t="s">
@@ -3596,16 +3614,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:N8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" style="25" bestFit="1" customWidth="1"/>
@@ -3627,35 +3645,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63" t="s">
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="60" t="s">
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="71" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="61"/>
-      <c r="T1" s="61"/>
-      <c r="U1" s="62"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="73"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3877,7 +3895,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="64" t="s">
+      <c r="J5" s="75" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -3944,7 +3962,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="64"/>
+      <c r="J6" s="75"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -4168,23 +4186,23 @@
       <c r="D10" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="74" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63" t="s">
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="63"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -4234,10 +4252,10 @@
       <c r="I11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="83" t="s">
         <v>130</v>
       </c>
       <c r="L11" s="20" t="s">
@@ -4249,7 +4267,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="64" t="s">
+      <c r="O11" s="75" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -4304,7 +4322,7 @@
         <v>96</v>
       </c>
       <c r="J12" s="21"/>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="80" t="s">
         <v>131</v>
       </c>
       <c r="L12" s="20" t="s">
@@ -4316,7 +4334,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="64"/>
+      <c r="O12" s="75"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -4352,7 +4370,7 @@
       <c r="D13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="53" t="s">
+      <c r="E13" s="51" t="s">
         <v>178</v>
       </c>
       <c r="F13" s="28" t="s">
@@ -4367,10 +4385,10 @@
       <c r="I13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="53" t="s">
+      <c r="J13" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="80" t="s">
         <v>132</v>
       </c>
       <c r="L13" s="20" t="s">
@@ -4382,7 +4400,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="64"/>
+      <c r="O13" s="75"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -4410,14 +4428,14 @@
         <v>104</v>
       </c>
       <c r="H14" s="20">
-        <f>H13*Parameters!C9*Parameters!C15/2</f>
+        <f>'General Calculations'!H13*Parameters!C9*Parameters!C15/2</f>
         <v>60</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>15</v>
       </c>
       <c r="J14" s="21"/>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="80" t="s">
         <v>135</v>
       </c>
       <c r="L14" s="20" t="s">
@@ -4464,7 +4482,7 @@
         <v>33</v>
       </c>
       <c r="J15" s="36"/>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="80" t="s">
         <v>145</v>
       </c>
       <c r="L15" s="20" t="s">
@@ -4476,7 +4494,7 @@
       <c r="N15" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="O15" s="53" t="s">
+      <c r="O15" s="51" t="s">
         <v>178</v>
       </c>
       <c r="R15" s="38"/>
@@ -4488,7 +4506,7 @@
       <c r="A16" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="53" t="s">
         <v>227</v>
       </c>
       <c r="C16" s="23">
@@ -4513,7 +4531,7 @@
         <v>33</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="83" t="s">
         <v>139</v>
       </c>
       <c r="L16" s="20" t="s">
@@ -4533,28 +4551,28 @@
       <c r="U16" s="38"/>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="56" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="53" t="s">
         <v>228</v>
       </c>
       <c r="C17" s="23">
-        <f>Parameters!H8*(C14-M14)/'General Calculations'!C3</f>
+        <f>Parameters!H8*(C14-M14)/C3</f>
         <v>33.171057287635783</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="63" t="s">
+      <c r="F17" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="29" t="s">
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="80" t="s">
         <v>140</v>
       </c>
       <c r="L17" s="20" t="s">
@@ -4574,7 +4592,7 @@
       <c r="U17" s="38"/>
     </row>
     <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="36" t="s">
         <v>214</v>
       </c>
       <c r="B18" s="20" t="s">
@@ -4602,7 +4620,7 @@
         <v>80</v>
       </c>
       <c r="J18" s="40"/>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="80" t="s">
         <v>137</v>
       </c>
       <c r="L18" s="20" t="s">
@@ -4652,7 +4670,7 @@
         <v>166</v>
       </c>
       <c r="J19" s="20"/>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="82" t="s">
         <v>146</v>
       </c>
       <c r="L19" s="20" t="s">
@@ -4664,7 +4682,7 @@
       <c r="N19" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O19" s="53" t="s">
+      <c r="O19" s="51" t="s">
         <v>178</v>
       </c>
       <c r="R19" s="38"/>
@@ -4673,15 +4691,15 @@
       <c r="U19" s="38"/>
     </row>
     <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="54" t="s">
         <v>235</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57">
+      <c r="B20" s="55"/>
+      <c r="C20" s="55">
         <f>C19*PI()/2/C18</f>
         <v>1.91468163484499</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="55" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="39"/>
@@ -4699,7 +4717,7 @@
         <v>7</v>
       </c>
       <c r="J20" s="20"/>
-      <c r="K20" s="41" t="s">
+      <c r="K20" s="82" t="s">
         <v>150</v>
       </c>
       <c r="L20" s="20" t="s">
@@ -4737,7 +4755,7 @@
         <v>7</v>
       </c>
       <c r="J21" s="20"/>
-      <c r="K21" s="42" t="s">
+      <c r="K21" s="82" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="22" t="s">
@@ -4778,10 +4796,10 @@
       <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="43" t="s">
         <v>197</v>
       </c>
       <c r="H23" s="20">
@@ -4791,22 +4809,22 @@
       <c r="I23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="46"/>
-      <c r="K23" s="63" t="s">
+      <c r="J23" s="44"/>
+      <c r="K23" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
+      <c r="L23" s="74"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="44"/>
-      <c r="G24" s="45"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="43"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="29" t="s">
+      <c r="J24" s="44"/>
+      <c r="K24" s="80" t="s">
         <v>198</v>
       </c>
       <c r="L24" s="20" t="s">
@@ -4822,12 +4840,12 @@
       <c r="O24" s="20"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="44"/>
-      <c r="G25" s="45"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="29" t="s">
+      <c r="J25" s="44"/>
+      <c r="K25" s="80" t="s">
         <v>198</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -4843,12 +4861,12 @@
       <c r="O25" s="20"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="44"/>
-      <c r="G26" s="45"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="29" t="s">
+      <c r="J26" s="44"/>
+      <c r="K26" s="80" t="s">
         <v>187</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -4868,8 +4886,8 @@
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
-      <c r="J27" s="46"/>
-      <c r="K27" s="29" t="s">
+      <c r="J27" s="44"/>
+      <c r="K27" s="80" t="s">
         <v>188</v>
       </c>
       <c r="L27" s="20" t="s">
@@ -4885,7 +4903,7 @@
       <c r="O27" s="20"/>
     </row>
     <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="80" t="s">
         <v>203</v>
       </c>
       <c r="L28" s="20" t="s">
@@ -4913,10 +4931,10 @@
       <c r="I29" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J29" s="51" t="s">
+      <c r="J29" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="K29" s="29" t="s">
+      <c r="K29" s="80" t="s">
         <v>205</v>
       </c>
       <c r="L29" s="20" t="s">
@@ -4948,10 +4966,10 @@
       <c r="I30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="51" t="s">
+      <c r="J30" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="80" t="s">
         <v>189</v>
       </c>
       <c r="L30" s="20" t="s">
@@ -4963,12 +4981,12 @@
       <c r="N30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="O30" s="53" t="s">
+      <c r="O30" s="51" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="47" t="s">
         <v>218</v>
       </c>
       <c r="G31" s="20" t="s">
@@ -4978,14 +4996,14 @@
         <v>0.95</v>
       </c>
       <c r="I31" s="40"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="29" t="s">
+      <c r="J31" s="41"/>
+      <c r="K31" s="80" t="s">
         <v>192</v>
       </c>
       <c r="L31" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="M31" s="47">
+      <c r="M31" s="45">
         <f>M30*Parameters!H11</f>
         <v>1.3823007660000001E-6</v>
       </c>
@@ -5005,8 +5023,8 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="I32" s="20"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="28" t="s">
+      <c r="J32" s="41"/>
+      <c r="K32" s="81" t="s">
         <v>207</v>
       </c>
       <c r="L32" s="20" t="s">
@@ -5018,7 +5036,7 @@
       <c r="N32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="O32" s="53" t="s">
+      <c r="O32" s="51" t="s">
         <v>178</v>
       </c>
     </row>
@@ -5027,8 +5045,8 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="28" t="s">
+      <c r="J33" s="41"/>
+      <c r="K33" s="81" t="s">
         <v>222</v>
       </c>
       <c r="L33" s="20" t="s">
@@ -5048,7 +5066,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="K34" s="28" t="s">
+      <c r="K34" s="81" t="s">
         <v>222</v>
       </c>
       <c r="L34" s="20" t="s">
@@ -5085,450 +5103,450 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="76" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4" style="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.7109375" style="76" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" style="76" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="76" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" style="76" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.5703125" style="76" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="75"/>
+    <col min="1" max="1" width="23" style="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="65" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" style="65" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5703125" style="65" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" style="65" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="64"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="76" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="78" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="77" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="61" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="69">
+      <c r="C2" s="60">
         <v>8000</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="79" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="H2" s="67">
+      <c r="H2" s="58">
         <f>C4/C5</f>
         <v>2</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="67"/>
+      <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="67">
+      <c r="C3" s="58">
         <v>540</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="79" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="H3" s="69">
+      <c r="H3" s="60">
         <f>C2/C4</f>
         <v>2000</v>
       </c>
-      <c r="I3" s="67" t="s">
+      <c r="I3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="67"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="58">
         <v>4</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="79" t="s">
+      <c r="E4" s="58"/>
+      <c r="F4" s="67" t="s">
         <v>250</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="H4" s="69">
+      <c r="H4" s="60">
         <f>H3/C9</f>
         <v>2298.8505747126437</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="58" t="s">
         <v>252</v>
       </c>
-      <c r="J4" s="67"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="67">
+      <c r="C5" s="58">
         <v>2</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="D5" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="79" t="s">
+      <c r="E5" s="58"/>
+      <c r="F5" s="67" t="s">
         <v>272</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="H5" s="69">
+      <c r="H5" s="60">
         <f>SQRT(H4^2-H3^2)</f>
         <v>1133.4522331605565</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="67"/>
+      <c r="J5" s="58"/>
     </row>
     <row r="6" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="58" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="67">
+      <c r="C6" s="58">
         <v>1</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="79" t="s">
+      <c r="E6" s="58"/>
+      <c r="F6" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G6" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="58">
         <f>C3/C5</f>
         <v>270</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="I6" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="67"/>
+      <c r="J6" s="58"/>
     </row>
     <row r="7" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="67">
+      <c r="C7" s="58">
         <v>3</v>
       </c>
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="79" t="s">
+      <c r="E7" s="58"/>
+      <c r="F7" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="58" t="s">
         <v>245</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="59">
         <f>0.612*C6*H6/SQRT(3)</f>
         <v>95.401358480893776</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="67"/>
+      <c r="J7" s="58"/>
     </row>
     <row r="8" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="58" t="s">
         <v>249</v>
       </c>
-      <c r="C8" s="67">
+      <c r="C8" s="58">
         <v>94</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="79" t="s">
+      <c r="E8" s="58"/>
+      <c r="F8" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="67" t="s">
+      <c r="G8" s="58" t="s">
         <v>247</v>
       </c>
-      <c r="H8" s="68">
+      <c r="H8" s="59">
         <f>H4/(C7*H7)</f>
         <v>8.0322076866198895</v>
       </c>
-      <c r="I8" s="67" t="s">
+      <c r="I8" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="67"/>
+      <c r="J8" s="58"/>
     </row>
     <row r="9" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="67">
+      <c r="C9" s="58">
         <v>0.87</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="58" t="s">
         <v>248</v>
       </c>
-      <c r="C10" s="67">
+      <c r="C10" s="58">
         <v>50</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="D10" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
     </row>
     <row r="11" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="61" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="C11" s="67">
+      <c r="C11" s="58">
         <v>5</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="D11" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-    </row>
-    <row r="12" spans="1:10" s="77" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+      <c r="E11" s="58"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+    </row>
+    <row r="12" spans="1:10" s="66" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="78" t="s">
         <v>256</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="65" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79" t="s">
         <v>256</v>
       </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
     </row>
     <row r="13" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="58" t="s">
         <v>255</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="59">
         <f>H7/H8</f>
         <v>11.877352056000003</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="81" t="s">
+      <c r="E13" s="58"/>
+      <c r="F13" s="69" t="s">
         <v>270</v>
       </c>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68">
+      <c r="G13" s="58"/>
+      <c r="H13" s="59">
         <f>C14*H8</f>
         <v>82.999181878377584</v>
       </c>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="59">
         <f>C13*C9</f>
         <v>10.333296288720003</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="81" t="s">
+      <c r="E14" s="58"/>
+      <c r="F14" s="69" t="s">
         <v>271</v>
       </c>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68">
+      <c r="G14" s="58"/>
+      <c r="H14" s="59">
         <f>C15*H8</f>
         <v>47.037804025273118</v>
       </c>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
     </row>
     <row r="15" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="63" t="s">
         <v>259</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="58" t="s">
         <v>260</v>
       </c>
-      <c r="C15" s="68">
+      <c r="C15" s="59">
         <f>SQRT(C13^2-C14^2)</f>
         <v>5.8561488771796872</v>
       </c>
-      <c r="D15" s="67" t="s">
+      <c r="D15" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
     </row>
     <row r="16" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="63" t="s">
         <v>261</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="58" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="59">
         <f>1000*C15/(2*3.14*C10)</f>
         <v>18.650155659807922</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
     </row>
     <row r="17" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="58" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="59">
         <f>C14*C11</f>
         <v>51.66648144360002</v>
       </c>
-      <c r="D17" s="67" t="s">
+      <c r="D17" s="58" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
     </row>
     <row r="18" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="58" t="s">
         <v>269</v>
       </c>
-      <c r="C18" s="68">
+      <c r="C18" s="59">
         <f>C16*C11</f>
         <v>93.250778299039609</v>
       </c>
-      <c r="D18" s="67" t="s">
+      <c r="D18" s="58" t="s">
         <v>263</v>
       </c>
-      <c r="E18" s="67"/>
+      <c r="E18" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5561,10 +5579,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="52" t="s">
         <v>230</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Design file continue with the aid of maxwell simulations. A fatal error is debugged and fixed (regarding fill factor). Most of the results are very similar and consistent. Still have a few things to fix.
</commit_message>
<xml_diff>
--- a/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
+++ b/Project/BAP/Design/Design report/Designfile.V1.0.xlsx
@@ -2709,6 +2709,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2738,18 +2750,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3379,12 +3379,12 @@
         <v>15</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="F7" s="70" t="s">
+      <c r="F7" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
@@ -3614,8 +3614,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,35 +3645,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74" t="s">
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="71" t="s">
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="75" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="73"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="77"/>
       <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3895,7 +3895,7 @@
       <c r="I5" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="79" t="s">
         <v>178</v>
       </c>
       <c r="K5" s="28" t="s">
@@ -3962,7 +3962,7 @@
       <c r="I6" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="75"/>
+      <c r="J6" s="79"/>
       <c r="K6" s="28" t="s">
         <v>26</v>
       </c>
@@ -4189,20 +4189,20 @@
       <c r="E10" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74" t="s">
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78"/>
       <c r="P10" s="31" t="s">
         <v>184</v>
       </c>
@@ -4255,7 +4255,7 @@
       <c r="J11" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="K11" s="83" t="s">
+      <c r="K11" s="73" t="s">
         <v>130</v>
       </c>
       <c r="L11" s="20" t="s">
@@ -4267,7 +4267,7 @@
       <c r="N11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O11" s="75" t="s">
+      <c r="O11" s="79" t="s">
         <v>178</v>
       </c>
       <c r="P11" s="31" t="s">
@@ -4322,7 +4322,7 @@
         <v>96</v>
       </c>
       <c r="J12" s="21"/>
-      <c r="K12" s="80" t="s">
+      <c r="K12" s="70" t="s">
         <v>131</v>
       </c>
       <c r="L12" s="20" t="s">
@@ -4334,7 +4334,7 @@
       <c r="N12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="75"/>
+      <c r="O12" s="79"/>
       <c r="P12" s="22" t="s">
         <v>1</v>
       </c>
@@ -4388,7 +4388,7 @@
       <c r="J13" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="K13" s="80" t="s">
+      <c r="K13" s="70" t="s">
         <v>132</v>
       </c>
       <c r="L13" s="20" t="s">
@@ -4400,7 +4400,7 @@
       <c r="N13" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="O13" s="75"/>
+      <c r="O13" s="79"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
       <c r="T13" s="38"/>
@@ -4435,7 +4435,7 @@
         <v>15</v>
       </c>
       <c r="J14" s="21"/>
-      <c r="K14" s="80" t="s">
+      <c r="K14" s="70" t="s">
         <v>135</v>
       </c>
       <c r="L14" s="20" t="s">
@@ -4482,7 +4482,7 @@
         <v>33</v>
       </c>
       <c r="J15" s="36"/>
-      <c r="K15" s="80" t="s">
+      <c r="K15" s="70" t="s">
         <v>145</v>
       </c>
       <c r="L15" s="20" t="s">
@@ -4531,7 +4531,7 @@
         <v>33</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="83" t="s">
+      <c r="K16" s="73" t="s">
         <v>139</v>
       </c>
       <c r="L16" s="20" t="s">
@@ -4565,14 +4565,14 @@
         <v>80</v>
       </c>
       <c r="E17" s="28"/>
-      <c r="F17" s="74" t="s">
+      <c r="F17" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="80" t="s">
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="70" t="s">
         <v>140</v>
       </c>
       <c r="L17" s="20" t="s">
@@ -4620,7 +4620,7 @@
         <v>80</v>
       </c>
       <c r="J18" s="40"/>
-      <c r="K18" s="80" t="s">
+      <c r="K18" s="70" t="s">
         <v>137</v>
       </c>
       <c r="L18" s="20" t="s">
@@ -4670,7 +4670,7 @@
         <v>166</v>
       </c>
       <c r="J19" s="20"/>
-      <c r="K19" s="82" t="s">
+      <c r="K19" s="72" t="s">
         <v>146</v>
       </c>
       <c r="L19" s="20" t="s">
@@ -4717,7 +4717,7 @@
         <v>7</v>
       </c>
       <c r="J20" s="20"/>
-      <c r="K20" s="82" t="s">
+      <c r="K20" s="72" t="s">
         <v>150</v>
       </c>
       <c r="L20" s="20" t="s">
@@ -4755,7 +4755,7 @@
         <v>7</v>
       </c>
       <c r="J21" s="20"/>
-      <c r="K21" s="82" t="s">
+      <c r="K21" s="72" t="s">
         <v>20</v>
       </c>
       <c r="L21" s="22" t="s">
@@ -4810,13 +4810,13 @@
         <v>15</v>
       </c>
       <c r="J23" s="44"/>
-      <c r="K23" s="74" t="s">
+      <c r="K23" s="78" t="s">
         <v>186</v>
       </c>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="42"/>
@@ -4824,7 +4824,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
       <c r="J24" s="44"/>
-      <c r="K24" s="80" t="s">
+      <c r="K24" s="70" t="s">
         <v>198</v>
       </c>
       <c r="L24" s="20" t="s">
@@ -4845,7 +4845,7 @@
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="44"/>
-      <c r="K25" s="80" t="s">
+      <c r="K25" s="70" t="s">
         <v>198</v>
       </c>
       <c r="L25" s="20" t="s">
@@ -4866,7 +4866,7 @@
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
       <c r="J26" s="44"/>
-      <c r="K26" s="80" t="s">
+      <c r="K26" s="70" t="s">
         <v>187</v>
       </c>
       <c r="L26" s="20" t="s">
@@ -4887,7 +4887,7 @@
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
       <c r="J27" s="44"/>
-      <c r="K27" s="80" t="s">
+      <c r="K27" s="70" t="s">
         <v>188</v>
       </c>
       <c r="L27" s="20" t="s">
@@ -4903,7 +4903,7 @@
       <c r="O27" s="20"/>
     </row>
     <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="80" t="s">
+      <c r="K28" s="70" t="s">
         <v>203</v>
       </c>
       <c r="L28" s="20" t="s">
@@ -4934,7 +4934,7 @@
       <c r="J29" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="K29" s="80" t="s">
+      <c r="K29" s="70" t="s">
         <v>205</v>
       </c>
       <c r="L29" s="20" t="s">
@@ -4969,7 +4969,7 @@
       <c r="J30" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="K30" s="80" t="s">
+      <c r="K30" s="70" t="s">
         <v>189</v>
       </c>
       <c r="L30" s="20" t="s">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="I31" s="40"/>
       <c r="J31" s="41"/>
-      <c r="K31" s="80" t="s">
+      <c r="K31" s="70" t="s">
         <v>192</v>
       </c>
       <c r="L31" s="20" t="s">
@@ -5024,7 +5024,7 @@
       </c>
       <c r="I32" s="20"/>
       <c r="J32" s="41"/>
-      <c r="K32" s="81" t="s">
+      <c r="K32" s="71" t="s">
         <v>207</v>
       </c>
       <c r="L32" s="20" t="s">
@@ -5046,7 +5046,7 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="41"/>
-      <c r="K33" s="81" t="s">
+      <c r="K33" s="71" t="s">
         <v>222</v>
       </c>
       <c r="L33" s="20" t="s">
@@ -5066,7 +5066,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
-      <c r="K34" s="81" t="s">
+      <c r="K34" s="71" t="s">
         <v>222</v>
       </c>
       <c r="L34" s="20" t="s">
@@ -5123,20 +5123,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="80" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="77" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="81" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
     </row>
     <row r="2" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="61" t="s">
@@ -5402,20 +5402,20 @@
       <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:10" s="66" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="82" t="s">
         <v>256</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79" t="s">
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">

</xml_diff>